<commit_message>
Upload slides estimacion MCO
</commit_message>
<xml_diff>
--- a/econometria_I/Cronograma_Econometria I_2025.xlsx
+++ b/econometria_I/Cronograma_Econometria I_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramirodeelejalde/Dropbox/Teaching/Econometria I_MAE/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2EB116-76ED-A445-905D-BA18052340DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBABD080-10FF-C445-8718-599702ACFD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="960" windowWidth="24860" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,16 +602,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -844,38 +844,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="29"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -885,7 +885,7 @@
         <v>45887</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C45" si="0">B3</f>
+        <f t="shared" ref="C3:C44" si="0">B3</f>
         <v>45887</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1174,25 +1174,25 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>6</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="4">
         <v>45922</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>45922</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11" t="s">
+      <c r="D19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
@@ -1205,7 +1205,7 @@
         <f t="shared" si="0"/>
         <v>45924</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="3"/>
@@ -1300,29 +1300,29 @@
       <c r="D25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="9">
         <v>8</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="10">
         <v>45938</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="11">
         <f t="shared" si="0"/>
         <v>45938</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5"/>
+      <c r="D26" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
@@ -1353,7 +1353,7 @@
         <f t="shared" si="0"/>
         <v>45943</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="9"/>
@@ -1631,7 +1631,7 @@
         <f t="shared" si="0"/>
         <v>45978</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="28" t="s">
         <v>32</v>
       </c>
       <c r="E43" s="3"/>
@@ -1649,7 +1649,7 @@
         <f t="shared" si="0"/>
         <v>45980</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="33" t="s">
         <v>32</v>
       </c>
       <c r="E44" s="3"/>
@@ -1695,22 +1695,22 @@
       <c r="G46" s="24"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="31">
+      <c r="A47" s="29">
         <v>15</v>
       </c>
-      <c r="B47" s="32">
+      <c r="B47" s="30">
         <v>45987</v>
       </c>
-      <c r="C47" s="33">
+      <c r="C47" s="31">
         <f t="shared" si="2"/>
         <v>45987</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="33"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21"/>

</xml_diff>